<commit_message>
Language and error handling fixes
</commit_message>
<xml_diff>
--- a/public/xls-template/Sammanställning_deltagare.xlsx
+++ b/public/xls-template/Sammanställning_deltagare.xlsx
@@ -2101,79 +2101,28 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2230,22 +2179,101 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2280,34 +2308,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="10"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3188,7 +3188,7 @@
   <dimension ref="A1:Y521"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,26 +3208,27 @@
     <col min="14" max="14" width="13.140625" customWidth="1"/>
     <col min="15" max="15" width="12.140625" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" customWidth="1"/>
     <col min="19" max="19" width="42" customWidth="1"/>
     <col min="20" max="20" width="12.28515625" customWidth="1"/>
     <col min="21" max="21" width="11.85546875" customWidth="1"/>
     <col min="22" max="22" width="15.7109375" customWidth="1"/>
     <col min="23" max="23" width="23" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="1.5703125" customWidth="1"/>
+    <col min="25" max="25" width="0.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="198" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="157"/>
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -3249,16 +3250,16 @@
       <c r="Y1" s="24"/>
     </row>
     <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="158" t="s">
+      <c r="A2" s="199" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="158"/>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="158"/>
-      <c r="G2" s="158"/>
-      <c r="H2" s="158"/>
+      <c r="B2" s="199"/>
+      <c r="C2" s="199"/>
+      <c r="D2" s="199"/>
+      <c r="E2" s="199"/>
+      <c r="F2" s="199"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="199"/>
       <c r="L2" s="25"/>
       <c r="M2" s="26"/>
       <c r="N2" s="24"/>
@@ -3277,11 +3278,11 @@
       <c r="A3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="159"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="161"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="202"/>
       <c r="G3" s="27" t="s">
         <v>41</v>
       </c>
@@ -3304,27 +3305,27 @@
       <c r="A4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="159"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="161"/>
+      <c r="B4" s="200"/>
+      <c r="C4" s="201"/>
+      <c r="D4" s="201"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="202"/>
       <c r="G4" s="27" t="s">
         <v>42</v>
       </c>
       <c r="H4" s="28"/>
-      <c r="L4" s="162" t="s">
+      <c r="L4" s="203" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="163"/>
+      <c r="M4" s="204"/>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30"/>
       <c r="Q4" s="30"/>
-      <c r="R4" s="168" t="s">
+      <c r="R4" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="168" t="s">
+      <c r="S4" s="183" t="s">
         <v>45</v>
       </c>
       <c r="T4" s="24"/>
@@ -3349,8 +3350,8 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="169"/>
-      <c r="S5" s="169"/>
+      <c r="R5" s="184"/>
+      <c r="S5" s="184"/>
       <c r="T5" s="30"/>
       <c r="U5" s="30"/>
       <c r="V5" s="30"/>
@@ -3360,8 +3361,8 @@
     </row>
     <row r="6" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
-      <c r="B6" s="170"/>
-      <c r="C6" s="170"/>
+      <c r="B6" s="185"/>
+      <c r="C6" s="185"/>
       <c r="D6" s="36"/>
       <c r="E6" s="36"/>
       <c r="F6" s="35"/>
@@ -3370,126 +3371,126 @@
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
-      <c r="L6" s="171" t="s">
+      <c r="L6" s="186" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="172"/>
-      <c r="N6" s="173" t="s">
+      <c r="M6" s="187"/>
+      <c r="N6" s="188" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="174"/>
-      <c r="P6" s="175"/>
-      <c r="Q6" s="176" t="s">
+      <c r="O6" s="189"/>
+      <c r="P6" s="190"/>
+      <c r="Q6" s="191" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="177"/>
-      <c r="S6" s="177"/>
-      <c r="T6" s="177"/>
-      <c r="U6" s="177"/>
-      <c r="V6" s="177"/>
-      <c r="W6" s="177"/>
-      <c r="X6" s="177"/>
-      <c r="Y6" s="178"/>
+      <c r="R6" s="192"/>
+      <c r="S6" s="192"/>
+      <c r="T6" s="192"/>
+      <c r="U6" s="192"/>
+      <c r="V6" s="192"/>
+      <c r="W6" s="192"/>
+      <c r="X6" s="192"/>
+      <c r="Y6" s="193"/>
     </row>
     <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="164" t="s">
+      <c r="A7" s="194" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="164" t="s">
+      <c r="B7" s="194" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="164" t="s">
+      <c r="C7" s="194" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="166" t="s">
+      <c r="D7" s="196" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="166" t="s">
+      <c r="E7" s="196" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="181" t="s">
+      <c r="F7" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="181" t="s">
+      <c r="G7" s="165" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="181" t="s">
+      <c r="H7" s="165" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="183" t="s">
+      <c r="I7" s="167" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="185" t="s">
+      <c r="J7" s="169" t="s">
         <v>57</v>
       </c>
       <c r="K7" s="38"/>
-      <c r="L7" s="187" t="s">
+      <c r="L7" s="171" t="s">
         <v>58</v>
       </c>
-      <c r="M7" s="189" t="s">
+      <c r="M7" s="173" t="s">
         <v>59</v>
       </c>
-      <c r="N7" s="191" t="s">
+      <c r="N7" s="175" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="193" t="s">
+      <c r="O7" s="177" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="195" t="s">
+      <c r="P7" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="Q7" s="197" t="s">
+      <c r="Q7" s="181" t="s">
         <v>63</v>
       </c>
-      <c r="R7" s="179" t="s">
+      <c r="R7" s="161" t="s">
         <v>64</v>
       </c>
-      <c r="S7" s="201" t="s">
+      <c r="S7" s="159" t="s">
         <v>65</v>
       </c>
-      <c r="T7" s="179" t="s">
+      <c r="T7" s="161" t="s">
         <v>66</v>
       </c>
-      <c r="U7" s="179" t="s">
+      <c r="U7" s="161" t="s">
         <v>67</v>
       </c>
-      <c r="V7" s="179" t="s">
+      <c r="V7" s="161" t="s">
         <v>68</v>
       </c>
-      <c r="W7" s="179" t="s">
+      <c r="W7" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="X7" s="203" t="s">
+      <c r="X7" s="163" t="s">
         <v>70</v>
       </c>
-      <c r="Y7" s="199"/>
+      <c r="Y7" s="157"/>
     </row>
     <row r="8" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="165"/>
-      <c r="B8" s="165"/>
-      <c r="C8" s="165"/>
-      <c r="D8" s="167"/>
-      <c r="E8" s="167"/>
-      <c r="F8" s="182"/>
-      <c r="G8" s="182"/>
-      <c r="H8" s="182"/>
-      <c r="I8" s="184"/>
-      <c r="J8" s="186"/>
+      <c r="A8" s="195"/>
+      <c r="B8" s="195"/>
+      <c r="C8" s="195"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="166"/>
+      <c r="H8" s="166"/>
+      <c r="I8" s="168"/>
+      <c r="J8" s="170"/>
       <c r="K8" s="39"/>
-      <c r="L8" s="188"/>
-      <c r="M8" s="190"/>
-      <c r="N8" s="192"/>
-      <c r="O8" s="194"/>
-      <c r="P8" s="196"/>
-      <c r="Q8" s="198"/>
-      <c r="R8" s="180"/>
-      <c r="S8" s="202"/>
-      <c r="T8" s="180"/>
-      <c r="U8" s="180"/>
-      <c r="V8" s="180"/>
-      <c r="W8" s="180"/>
-      <c r="X8" s="204"/>
-      <c r="Y8" s="200"/>
+      <c r="L8" s="172"/>
+      <c r="M8" s="174"/>
+      <c r="N8" s="176"/>
+      <c r="O8" s="178"/>
+      <c r="P8" s="180"/>
+      <c r="Q8" s="182"/>
+      <c r="R8" s="162"/>
+      <c r="S8" s="160"/>
+      <c r="T8" s="162"/>
+      <c r="U8" s="162"/>
+      <c r="V8" s="162"/>
+      <c r="W8" s="162"/>
+      <c r="X8" s="164"/>
+      <c r="Y8" s="158"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="40"/>
@@ -28095,13 +28096,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:Y6"/>
+    <mergeCell ref="R4:R5"/>
     <mergeCell ref="R7:R8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
@@ -28114,22 +28124,13 @@
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="P7:P8"/>
     <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:Y6"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="X7:X8"/>
   </mergeCells>
   <dataValidations count="29">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Besvaras bara med Ja eller Nej" promptTitle="Kvalifikation" prompt="Läs instruktion för kvalifikation. Välj om deltagare erhållit någon formell kvalifikation." sqref="S10 S42 S74 S106 S138 S170 S202 S234 S266 S298 S330 S362 S394 S426 S458 S490">
@@ -28250,29 +28251,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="205" t="s">
+      <c r="A1" s="214" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
+      <c r="B1" s="214"/>
+      <c r="C1" s="214"/>
+      <c r="D1" s="214"/>
+      <c r="E1" s="214"/>
     </row>
     <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="205"/>
-      <c r="B2" s="205"/>
-      <c r="C2" s="205"/>
-      <c r="D2" s="205"/>
-      <c r="E2" s="205"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
+      <c r="C2" s="214"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="206" t="s">
+      <c r="A3" s="215" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="206"/>
-      <c r="C3" s="206"/>
-      <c r="D3" s="206"/>
-      <c r="E3" s="206"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="119"/>
@@ -28351,12 +28352,12 @@
       <c r="E11" s="128"/>
     </row>
     <row r="12" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="207" t="s">
+      <c r="A12" s="216" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="208"/>
-      <c r="C12" s="208"/>
-      <c r="D12" s="209"/>
+      <c r="B12" s="217"/>
+      <c r="C12" s="217"/>
+      <c r="D12" s="218"/>
       <c r="E12" s="121"/>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -28366,22 +28367,22 @@
       <c r="B13" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="210" t="s">
+      <c r="C13" s="219" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="211"/>
+      <c r="D13" s="220"/>
       <c r="E13" s="121"/>
     </row>
     <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="212" t="s">
+      <c r="A14" s="221" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="213"/>
-      <c r="C14" s="214">
+      <c r="B14" s="222"/>
+      <c r="C14" s="223">
         <f>Deltagarförteckning!H41</f>
         <v>0</v>
       </c>
-      <c r="D14" s="215"/>
+      <c r="D14" s="224"/>
       <c r="E14" s="121"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -28399,10 +28400,10 @@
       <c r="E16" s="121"/>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="216" t="s">
+      <c r="A17" s="207" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="216"/>
+      <c r="B17" s="207"/>
       <c r="C17" s="133">
         <f>COUNTIF(Deltagarförteckning!M9:M400,"&gt;0")</f>
         <v>0</v>
@@ -28411,10 +28412,10 @@
       <c r="E17" s="121"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="216" t="s">
+      <c r="A18" s="207" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="216"/>
+      <c r="B18" s="207"/>
       <c r="C18" s="133" t="str">
         <f>Deltagarförteckning!J41</f>
         <v/>
@@ -28423,10 +28424,10 @@
       <c r="E18" s="121"/>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="217" t="s">
+      <c r="A19" s="212" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="217"/>
+      <c r="B19" s="212"/>
       <c r="C19" s="133">
         <f>SUM(Deltagarförteckning!H41)</f>
         <v>0</v>
@@ -28435,17 +28436,17 @@
       <c r="E19" s="121"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="218"/>
-      <c r="B20" s="218"/>
-      <c r="C20" s="218"/>
-      <c r="D20" s="218"/>
+      <c r="A20" s="213"/>
+      <c r="B20" s="213"/>
+      <c r="C20" s="213"/>
+      <c r="D20" s="213"/>
       <c r="E20" s="121"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="217" t="s">
+      <c r="A21" s="212" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="217"/>
+      <c r="B21" s="212"/>
       <c r="C21" s="134" t="str">
         <f>IFERROR(C19/C17,"")</f>
         <v/>
@@ -28454,10 +28455,10 @@
       <c r="E21" s="121"/>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="217" t="s">
+      <c r="A22" s="212" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="217"/>
+      <c r="B22" s="212"/>
       <c r="C22" s="134" t="str">
         <f>IFERROR(C19/C18,"")</f>
         <v/>
@@ -28466,10 +28467,10 @@
       <c r="E22" s="121"/>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="216" t="s">
+      <c r="A23" s="207" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="216"/>
+      <c r="B23" s="207"/>
       <c r="C23" s="135">
         <f>COUNTIF(Deltagarförteckning!E9:E500,"=K")</f>
         <v>0</v>
@@ -28478,10 +28479,10 @@
       <c r="E23" s="121"/>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="216" t="s">
+      <c r="A24" s="207" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="216"/>
+      <c r="B24" s="207"/>
       <c r="C24" s="135">
         <f>COUNTIF(Deltagarförteckning!E9:E500,"=M")</f>
         <v>0</v>
@@ -28499,10 +28500,10 @@
       <c r="E25" s="121"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="216" t="s">
+      <c r="A26" s="207" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="216"/>
+      <c r="B26" s="207"/>
       <c r="C26" s="135" t="str">
         <f ca="1">IF(Data!J1=0,"",Data!J1)</f>
         <v/>
@@ -28511,10 +28512,10 @@
       <c r="E26" s="121"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="216" t="s">
+      <c r="A27" s="207" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="216"/>
+      <c r="B27" s="207"/>
       <c r="C27" s="135" t="str">
         <f>IF(Data!J2=0,"",Data!J2)</f>
         <v/>
@@ -28523,10 +28524,10 @@
       <c r="E27" s="121"/>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="216" t="s">
+      <c r="A28" s="207" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="216"/>
+      <c r="B28" s="207"/>
       <c r="C28" s="135" t="str">
         <f>IF(Data!J3=0,"",Data!J3)</f>
         <v/>
@@ -28535,10 +28536,10 @@
       <c r="E28" s="121"/>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="216" t="s">
+      <c r="A29" s="207" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="216"/>
+      <c r="B29" s="207"/>
       <c r="C29" s="135" t="str">
         <f>IF(Data!J4=0,"",Data!J4)</f>
         <v/>
@@ -28547,10 +28548,10 @@
       <c r="E29" s="121"/>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="216" t="s">
+      <c r="A30" s="207" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="216"/>
+      <c r="B30" s="207"/>
       <c r="C30" s="135" t="str">
         <f>IF(Data!J5=0,"",Data!J5)</f>
         <v/>
@@ -28559,10 +28560,10 @@
       <c r="E30" s="121"/>
     </row>
     <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="216" t="s">
+      <c r="A31" s="207" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="216"/>
+      <c r="B31" s="207"/>
       <c r="C31" s="135" t="str">
         <f>IF(Data!J6=0,"",Data!J6)</f>
         <v/>
@@ -28571,10 +28572,10 @@
       <c r="E31" s="121"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="216" t="s">
+      <c r="A32" s="207" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="216"/>
+      <c r="B32" s="207"/>
       <c r="C32" s="135" t="str">
         <f>IF(Data!J7=0,"",Data!J7)</f>
         <v/>
@@ -28593,12 +28594,12 @@
       <c r="E33" s="121"/>
     </row>
     <row r="34" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="221" t="s">
+      <c r="A34" s="208" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="221"/>
-      <c r="C34" s="221"/>
-      <c r="D34" s="221"/>
+      <c r="B34" s="208"/>
+      <c r="C34" s="208"/>
+      <c r="D34" s="208"/>
       <c r="E34" s="143"/>
       <c r="F34" s="144"/>
       <c r="G34" s="144"/>
@@ -28622,28 +28623,28 @@
         <v>89</v>
       </c>
       <c r="B37" s="121"/>
-      <c r="C37" s="222" t="s">
+      <c r="C37" s="209" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="222"/>
+      <c r="D37" s="209"/>
       <c r="E37" s="121"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="223" t="s">
+      <c r="A38" s="210" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="223"/>
-      <c r="C38" s="224" t="s">
+      <c r="B38" s="210"/>
+      <c r="C38" s="211" t="s">
         <v>92</v>
       </c>
-      <c r="D38" s="224"/>
+      <c r="D38" s="211"/>
       <c r="E38" s="121"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="219" t="s">
+      <c r="A39" s="205" t="s">
         <v>93</v>
       </c>
-      <c r="B39" s="219"/>
+      <c r="B39" s="205"/>
       <c r="C39" s="121"/>
       <c r="D39" s="121"/>
       <c r="E39" s="121"/>
@@ -28663,27 +28664,27 @@
       <c r="E41" s="121"/>
     </row>
     <row r="42" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="220" t="s">
+      <c r="A42" s="206" t="s">
         <v>94</v>
       </c>
-      <c r="B42" s="220"/>
-      <c r="C42" s="220"/>
-      <c r="D42" s="220"/>
+      <c r="B42" s="206"/>
+      <c r="C42" s="206"/>
+      <c r="D42" s="206"/>
       <c r="E42" s="148"/>
       <c r="F42" s="149"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="220"/>
-      <c r="B43" s="220"/>
-      <c r="C43" s="220"/>
-      <c r="D43" s="220"/>
+      <c r="A43" s="206"/>
+      <c r="B43" s="206"/>
+      <c r="C43" s="206"/>
+      <c r="D43" s="206"/>
       <c r="E43" s="121"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="220"/>
-      <c r="B44" s="220"/>
-      <c r="C44" s="220"/>
-      <c r="D44" s="220"/>
+      <c r="A44" s="206"/>
+      <c r="B44" s="206"/>
+      <c r="C44" s="206"/>
+      <c r="D44" s="206"/>
       <c r="E44" s="121"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -28739,15 +28740,12 @@
   </sheetData>
   <sheetProtection password="C544" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="27">
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A42:D44"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
@@ -28760,12 +28758,15 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A42:D44"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Projektrelaterad tid" error="- Bara projektrelaterade timmar registreras i blanketten. _x000a__x000a_Klicka på avbryt eller försök igen för att gå tillbaka och ändra._x000a_" sqref="C17 C33"/>

</xml_diff>

<commit_message>
One last wron formula in Excel file
</commit_message>
<xml_diff>
--- a/public/xls-template/Sammanställning_deltagare.xlsx
+++ b/public/xls-template/Sammanställning_deltagare.xlsx
@@ -2008,71 +2008,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2134,10 +2074,98 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2172,34 +2200,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="10"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3079,8 +3079,8 @@
   </sheetPr>
   <dimension ref="A1:V1010"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView topLeftCell="A973" workbookViewId="0">
+      <selection activeCell="H1010" sqref="H1010"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3108,16 +3108,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="181" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -3136,16 +3136,16 @@
       <c r="V1" s="23"/>
     </row>
     <row r="2" spans="1:22" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="182" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
+      <c r="B2" s="182"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
       <c r="L2" s="25"/>
       <c r="M2" s="26"/>
       <c r="N2" s="24"/>
@@ -3162,11 +3162,11 @@
       <c r="A3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="147"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="149"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="185"/>
       <c r="G3" s="27" t="s">
         <v>41</v>
       </c>
@@ -3187,27 +3187,27 @@
       <c r="A4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="147"/>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="149"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="184"/>
+      <c r="D4" s="184"/>
+      <c r="E4" s="184"/>
+      <c r="F4" s="185"/>
       <c r="G4" s="27" t="s">
         <v>42</v>
       </c>
       <c r="H4" s="28"/>
-      <c r="L4" s="150" t="s">
+      <c r="L4" s="186" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="151"/>
+      <c r="M4" s="187"/>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30"/>
       <c r="Q4" s="30"/>
-      <c r="R4" s="156" t="s">
+      <c r="R4" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="156" t="s">
+      <c r="S4" s="167" t="s">
         <v>45</v>
       </c>
       <c r="T4" s="24"/>
@@ -3229,16 +3229,16 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="157"/>
-      <c r="S5" s="157"/>
+      <c r="R5" s="168"/>
+      <c r="S5" s="168"/>
       <c r="T5" s="30"/>
       <c r="U5" s="30"/>
       <c r="V5" s="30"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
-      <c r="B6" s="158"/>
-      <c r="C6" s="158"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="169"/>
       <c r="D6" s="36"/>
       <c r="E6" s="36"/>
       <c r="F6" s="35"/>
@@ -3247,113 +3247,113 @@
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
-      <c r="L6" s="159" t="s">
+      <c r="L6" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="160"/>
-      <c r="N6" s="161" t="s">
+      <c r="M6" s="171"/>
+      <c r="N6" s="172" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="162"/>
-      <c r="P6" s="163"/>
-      <c r="Q6" s="164" t="s">
+      <c r="O6" s="173"/>
+      <c r="P6" s="174"/>
+      <c r="Q6" s="175" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="165"/>
-      <c r="S6" s="165"/>
-      <c r="T6" s="165"/>
-      <c r="U6" s="165"/>
-      <c r="V6" s="165"/>
+      <c r="R6" s="176"/>
+      <c r="S6" s="176"/>
+      <c r="T6" s="176"/>
+      <c r="U6" s="176"/>
+      <c r="V6" s="176"/>
     </row>
     <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="152" t="s">
+      <c r="A7" s="177" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="152" t="s">
+      <c r="B7" s="177" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="152" t="s">
+      <c r="C7" s="177" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="154" t="s">
+      <c r="D7" s="179" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="154" t="s">
+      <c r="E7" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="168" t="s">
+      <c r="F7" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="168" t="s">
+      <c r="G7" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="168" t="s">
+      <c r="H7" s="149" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="170" t="s">
+      <c r="I7" s="151" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="172" t="s">
+      <c r="J7" s="153" t="s">
         <v>57</v>
       </c>
       <c r="K7" s="38"/>
-      <c r="L7" s="174" t="s">
+      <c r="L7" s="155" t="s">
         <v>58</v>
       </c>
-      <c r="M7" s="176" t="s">
+      <c r="M7" s="157" t="s">
         <v>59</v>
       </c>
-      <c r="N7" s="178" t="s">
+      <c r="N7" s="159" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="180" t="s">
+      <c r="O7" s="161" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="182" t="s">
+      <c r="P7" s="163" t="s">
         <v>62</v>
       </c>
-      <c r="Q7" s="184" t="s">
+      <c r="Q7" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="R7" s="166" t="s">
+      <c r="R7" s="147" t="s">
         <v>64</v>
       </c>
-      <c r="S7" s="186" t="s">
+      <c r="S7" s="145" t="s">
         <v>65</v>
       </c>
-      <c r="T7" s="166" t="s">
+      <c r="T7" s="147" t="s">
         <v>66</v>
       </c>
-      <c r="U7" s="166" t="s">
+      <c r="U7" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="V7" s="166" t="s">
+      <c r="V7" s="147" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="153"/>
-      <c r="B8" s="153"/>
-      <c r="C8" s="153"/>
-      <c r="D8" s="155"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="169"/>
-      <c r="H8" s="169"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="173"/>
+      <c r="A8" s="178"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="178"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="150"/>
+      <c r="G8" s="150"/>
+      <c r="H8" s="150"/>
+      <c r="I8" s="152"/>
+      <c r="J8" s="154"/>
       <c r="K8" s="39"/>
-      <c r="L8" s="175"/>
-      <c r="M8" s="177"/>
-      <c r="N8" s="179"/>
-      <c r="O8" s="181"/>
-      <c r="P8" s="183"/>
-      <c r="Q8" s="185"/>
-      <c r="R8" s="167"/>
-      <c r="S8" s="187"/>
-      <c r="T8" s="167"/>
-      <c r="U8" s="167"/>
-      <c r="V8" s="167"/>
+      <c r="L8" s="156"/>
+      <c r="M8" s="158"/>
+      <c r="N8" s="160"/>
+      <c r="O8" s="162"/>
+      <c r="P8" s="164"/>
+      <c r="Q8" s="166"/>
+      <c r="R8" s="148"/>
+      <c r="S8" s="146"/>
+      <c r="T8" s="148"/>
+      <c r="U8" s="148"/>
+      <c r="V8" s="148"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="40"/>
@@ -48411,7 +48411,7 @@
       <c r="F1010" s="100"/>
       <c r="G1010" s="100"/>
       <c r="H1010" s="101">
-        <f>SUM(H9:H39)</f>
+        <f>SUM(H9:H1009)</f>
         <v>0</v>
       </c>
       <c r="I1010" s="102"/>
@@ -48428,21 +48428,16 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="S4:S5"/>
     <mergeCell ref="B6:C6"/>
@@ -48450,16 +48445,21 @@
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="Q6:V6"/>
     <mergeCell ref="R4:R5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="R7:R8"/>
   </mergeCells>
   <dataValidations count="26">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Besvaras bara med Ja eller Nej" promptTitle="Kvalifikation" prompt="Läs instruktion för kvalifikation. Välj om deltagare erhållit någon formell kvalifikation." sqref="S10 S40 S70 S100 S130 S160 S190 S220 S250 S381 S411 S441 S471 S501 S531 S561 S590 S636 S665 S292 S322 S352 S713 S743 S773 S803 S833 S863 S892 S938 S967">
@@ -48574,29 +48574,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="197" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
     </row>
     <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="188"/>
-      <c r="B2" s="188"/>
-      <c r="C2" s="188"/>
-      <c r="D2" s="188"/>
-      <c r="E2" s="188"/>
+      <c r="A2" s="197"/>
+      <c r="B2" s="197"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="198" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="189"/>
-      <c r="C3" s="189"/>
-      <c r="D3" s="189"/>
-      <c r="E3" s="189"/>
+      <c r="B3" s="198"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="198"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="107"/>
@@ -48675,12 +48675,12 @@
       <c r="E11" s="116"/>
     </row>
     <row r="12" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="190" t="s">
+      <c r="A12" s="199" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="191"/>
-      <c r="C12" s="191"/>
-      <c r="D12" s="192"/>
+      <c r="B12" s="200"/>
+      <c r="C12" s="200"/>
+      <c r="D12" s="201"/>
       <c r="E12" s="109"/>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -48690,22 +48690,22 @@
       <c r="B13" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="193" t="s">
+      <c r="C13" s="202" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="194"/>
+      <c r="D13" s="203"/>
       <c r="E13" s="109"/>
     </row>
     <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="195" t="s">
+      <c r="A14" s="204" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="196"/>
-      <c r="C14" s="197">
+      <c r="B14" s="205"/>
+      <c r="C14" s="206">
         <f>Deltagarförteckning!H1010</f>
         <v>0</v>
       </c>
-      <c r="D14" s="198"/>
+      <c r="D14" s="207"/>
       <c r="E14" s="109"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -48723,10 +48723,10 @@
       <c r="E16" s="109"/>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="199" t="s">
+      <c r="A17" s="190" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="199"/>
+      <c r="B17" s="190"/>
       <c r="C17" s="121">
         <f>COUNTIF(Deltagarförteckning!M9:M1009,"&gt;0")</f>
         <v>0</v>
@@ -48735,10 +48735,10 @@
       <c r="E17" s="109"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="199" t="s">
+      <c r="A18" s="190" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="199"/>
+      <c r="B18" s="190"/>
       <c r="C18" s="121">
         <f>Deltagarförteckning!J1010</f>
         <v>0</v>
@@ -48747,10 +48747,10 @@
       <c r="E18" s="109"/>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="200" t="s">
+      <c r="A19" s="195" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="200"/>
+      <c r="B19" s="195"/>
       <c r="C19" s="121">
         <f>SUM(Deltagarförteckning!H1010)</f>
         <v>0</v>
@@ -48759,17 +48759,17 @@
       <c r="E19" s="109"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="201"/>
-      <c r="B20" s="201"/>
-      <c r="C20" s="201"/>
-      <c r="D20" s="201"/>
+      <c r="A20" s="196"/>
+      <c r="B20" s="196"/>
+      <c r="C20" s="196"/>
+      <c r="D20" s="196"/>
       <c r="E20" s="109"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="200" t="s">
+      <c r="A21" s="195" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="200"/>
+      <c r="B21" s="195"/>
       <c r="C21" s="122" t="str">
         <f>IFERROR(C19/C17,"")</f>
         <v/>
@@ -48778,10 +48778,10 @@
       <c r="E21" s="109"/>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="200" t="s">
+      <c r="A22" s="195" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="200"/>
+      <c r="B22" s="195"/>
       <c r="C22" s="122" t="str">
         <f>IFERROR(C19/C18,"")</f>
         <v/>
@@ -48790,10 +48790,10 @@
       <c r="E22" s="109"/>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="199" t="s">
+      <c r="A23" s="190" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="199"/>
+      <c r="B23" s="190"/>
       <c r="C23" s="123">
         <f>COUNTIF(Deltagarförteckning!E9:E1009,"=K")</f>
         <v>0</v>
@@ -48802,10 +48802,10 @@
       <c r="E23" s="109"/>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="199" t="s">
+      <c r="A24" s="190" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="199"/>
+      <c r="B24" s="190"/>
       <c r="C24" s="123">
         <f>COUNTIF(Deltagarförteckning!E9:E1009,"=M")</f>
         <v>0</v>
@@ -48823,10 +48823,10 @@
       <c r="E25" s="109"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="199" t="s">
+      <c r="A26" s="190" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="199"/>
+      <c r="B26" s="190"/>
       <c r="C26" s="123" t="str">
         <f ca="1">IF(Data!J1=0,"",Data!J1)</f>
         <v/>
@@ -48835,10 +48835,10 @@
       <c r="E26" s="109"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="199" t="s">
+      <c r="A27" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="199"/>
+      <c r="B27" s="190"/>
       <c r="C27" s="123" t="str">
         <f>IF(Data!J2=0,"",Data!J2)</f>
         <v/>
@@ -48847,10 +48847,10 @@
       <c r="E27" s="109"/>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="199" t="s">
+      <c r="A28" s="190" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="199"/>
+      <c r="B28" s="190"/>
       <c r="C28" s="123" t="str">
         <f>IF(Data!J3=0,"",Data!J3)</f>
         <v/>
@@ -48859,10 +48859,10 @@
       <c r="E28" s="109"/>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="199" t="s">
+      <c r="A29" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="199"/>
+      <c r="B29" s="190"/>
       <c r="C29" s="123" t="str">
         <f>IF(Data!J4=0,"",Data!J4)</f>
         <v/>
@@ -48871,10 +48871,10 @@
       <c r="E29" s="109"/>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="199" t="s">
+      <c r="A30" s="190" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="199"/>
+      <c r="B30" s="190"/>
       <c r="C30" s="123" t="str">
         <f>IF(Data!J5=0,"",Data!J5)</f>
         <v/>
@@ -48883,10 +48883,10 @@
       <c r="E30" s="109"/>
     </row>
     <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="199" t="s">
+      <c r="A31" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="199"/>
+      <c r="B31" s="190"/>
       <c r="C31" s="123" t="str">
         <f>IF(Data!J6=0,"",Data!J6)</f>
         <v/>
@@ -48895,10 +48895,10 @@
       <c r="E31" s="109"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="199" t="s">
+      <c r="A32" s="190" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="199"/>
+      <c r="B32" s="190"/>
       <c r="C32" s="123" t="str">
         <f>IF(Data!J7=0,"",Data!J7)</f>
         <v/>
@@ -48917,12 +48917,12 @@
       <c r="E33" s="109"/>
     </row>
     <row r="34" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="204" t="s">
+      <c r="A34" s="191" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="204"/>
-      <c r="C34" s="204"/>
-      <c r="D34" s="204"/>
+      <c r="B34" s="191"/>
+      <c r="C34" s="191"/>
+      <c r="D34" s="191"/>
       <c r="E34" s="131"/>
       <c r="F34" s="132"/>
       <c r="G34" s="132"/>
@@ -48946,28 +48946,28 @@
         <v>87</v>
       </c>
       <c r="B37" s="109"/>
-      <c r="C37" s="205" t="s">
+      <c r="C37" s="192" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="205"/>
+      <c r="D37" s="192"/>
       <c r="E37" s="109"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="206" t="s">
+      <c r="A38" s="193" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="206"/>
-      <c r="C38" s="207" t="s">
+      <c r="B38" s="193"/>
+      <c r="C38" s="194" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="207"/>
+      <c r="D38" s="194"/>
       <c r="E38" s="109"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="202" t="s">
+      <c r="A39" s="188" t="s">
         <v>91</v>
       </c>
-      <c r="B39" s="202"/>
+      <c r="B39" s="188"/>
       <c r="C39" s="109"/>
       <c r="D39" s="109"/>
       <c r="E39" s="109"/>
@@ -48987,27 +48987,27 @@
       <c r="E41" s="109"/>
     </row>
     <row r="42" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="203" t="s">
+      <c r="A42" s="189" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="203"/>
-      <c r="C42" s="203"/>
-      <c r="D42" s="203"/>
+      <c r="B42" s="189"/>
+      <c r="C42" s="189"/>
+      <c r="D42" s="189"/>
       <c r="E42" s="136"/>
       <c r="F42" s="137"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="203"/>
-      <c r="B43" s="203"/>
-      <c r="C43" s="203"/>
-      <c r="D43" s="203"/>
+      <c r="A43" s="189"/>
+      <c r="B43" s="189"/>
+      <c r="C43" s="189"/>
+      <c r="D43" s="189"/>
       <c r="E43" s="109"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="203"/>
-      <c r="B44" s="203"/>
-      <c r="C44" s="203"/>
-      <c r="D44" s="203"/>
+      <c r="A44" s="189"/>
+      <c r="B44" s="189"/>
+      <c r="C44" s="189"/>
+      <c r="D44" s="189"/>
       <c r="E44" s="109"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -49062,15 +49062,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A42:D44"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
@@ -49083,12 +49080,15 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A42:D44"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Projektrelaterad tid" error="- Bara projektrelaterade timmar registreras i blanketten. _x000a__x000a_Klicka på avbryt eller försök igen för att gå tillbaka och ändra._x000a_" sqref="C17 C33"/>

</xml_diff>

<commit_message>
Removed more stupid ESF stuff from Excel file
</commit_message>
<xml_diff>
--- a/public/xls-template/Sammanställning_deltagare.xlsx
+++ b/public/xls-template/Sammanställning_deltagare.xlsx
@@ -2008,65 +2008,41 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2104,68 +2080,64 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="10"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2200,6 +2172,34 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3108,16 +3108,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="181" t="s">
+      <c r="A1" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="181"/>
-      <c r="G1" s="181"/>
-      <c r="H1" s="181"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -3136,16 +3136,16 @@
       <c r="V1" s="23"/>
     </row>
     <row r="2" spans="1:22" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="146" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
       <c r="L2" s="25"/>
       <c r="M2" s="26"/>
       <c r="N2" s="24"/>
@@ -3162,11 +3162,11 @@
       <c r="A3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="185"/>
+      <c r="B3" s="147"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="149"/>
       <c r="G3" s="27" t="s">
         <v>41</v>
       </c>
@@ -3187,27 +3187,27 @@
       <c r="A4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="183"/>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="185"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="148"/>
+      <c r="D4" s="148"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="149"/>
       <c r="G4" s="27" t="s">
         <v>42</v>
       </c>
       <c r="H4" s="28"/>
-      <c r="L4" s="186" t="s">
+      <c r="L4" s="150" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="187"/>
+      <c r="M4" s="151"/>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30"/>
       <c r="Q4" s="30"/>
-      <c r="R4" s="167" t="s">
+      <c r="R4" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="167" t="s">
+      <c r="S4" s="158" t="s">
         <v>45</v>
       </c>
       <c r="T4" s="24"/>
@@ -3229,16 +3229,16 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="168"/>
-      <c r="S5" s="168"/>
+      <c r="R5" s="159"/>
+      <c r="S5" s="159"/>
       <c r="T5" s="30"/>
       <c r="U5" s="30"/>
       <c r="V5" s="30"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="169"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="160"/>
       <c r="D6" s="36"/>
       <c r="E6" s="36"/>
       <c r="F6" s="35"/>
@@ -3247,113 +3247,113 @@
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
-      <c r="L6" s="170" t="s">
+      <c r="L6" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="171"/>
-      <c r="N6" s="172" t="s">
+      <c r="M6" s="162"/>
+      <c r="N6" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="173"/>
-      <c r="P6" s="174"/>
-      <c r="Q6" s="175" t="s">
+      <c r="O6" s="164"/>
+      <c r="P6" s="165"/>
+      <c r="Q6" s="166" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="176"/>
-      <c r="S6" s="176"/>
-      <c r="T6" s="176"/>
-      <c r="U6" s="176"/>
-      <c r="V6" s="176"/>
+      <c r="R6" s="167"/>
+      <c r="S6" s="167"/>
+      <c r="T6" s="167"/>
+      <c r="U6" s="167"/>
+      <c r="V6" s="167"/>
     </row>
     <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="177" t="s">
+      <c r="A7" s="152" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="152" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="177" t="s">
+      <c r="C7" s="152" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="179" t="s">
+      <c r="D7" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="179" t="s">
+      <c r="E7" s="154" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="149" t="s">
+      <c r="F7" s="178" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="149" t="s">
+      <c r="G7" s="178" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="149" t="s">
+      <c r="H7" s="178" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="151" t="s">
+      <c r="I7" s="180" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="153" t="s">
+      <c r="J7" s="182" t="s">
         <v>57</v>
       </c>
       <c r="K7" s="38"/>
-      <c r="L7" s="155" t="s">
+      <c r="L7" s="168" t="s">
         <v>58</v>
       </c>
-      <c r="M7" s="157" t="s">
+      <c r="M7" s="170" t="s">
         <v>59</v>
       </c>
-      <c r="N7" s="159" t="s">
+      <c r="N7" s="172" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="161" t="s">
+      <c r="O7" s="174" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="163" t="s">
+      <c r="P7" s="176" t="s">
         <v>62</v>
       </c>
-      <c r="Q7" s="165" t="s">
+      <c r="Q7" s="156" t="s">
         <v>63</v>
       </c>
-      <c r="R7" s="147" t="s">
+      <c r="R7" s="186" t="s">
         <v>64</v>
       </c>
-      <c r="S7" s="145" t="s">
+      <c r="S7" s="184" t="s">
         <v>65</v>
       </c>
-      <c r="T7" s="147" t="s">
+      <c r="T7" s="186" t="s">
         <v>66</v>
       </c>
-      <c r="U7" s="147" t="s">
+      <c r="U7" s="186" t="s">
         <v>67</v>
       </c>
-      <c r="V7" s="147" t="s">
+      <c r="V7" s="186" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="178"/>
-      <c r="B8" s="178"/>
-      <c r="C8" s="178"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="150"/>
-      <c r="G8" s="150"/>
-      <c r="H8" s="150"/>
-      <c r="I8" s="152"/>
-      <c r="J8" s="154"/>
+      <c r="A8" s="153"/>
+      <c r="B8" s="153"/>
+      <c r="C8" s="153"/>
+      <c r="D8" s="155"/>
+      <c r="E8" s="155"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="179"/>
+      <c r="H8" s="179"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="183"/>
       <c r="K8" s="39"/>
-      <c r="L8" s="156"/>
-      <c r="M8" s="158"/>
-      <c r="N8" s="160"/>
-      <c r="O8" s="162"/>
-      <c r="P8" s="164"/>
-      <c r="Q8" s="166"/>
-      <c r="R8" s="148"/>
-      <c r="S8" s="146"/>
-      <c r="T8" s="148"/>
-      <c r="U8" s="148"/>
-      <c r="V8" s="148"/>
+      <c r="L8" s="169"/>
+      <c r="M8" s="171"/>
+      <c r="N8" s="173"/>
+      <c r="O8" s="175"/>
+      <c r="P8" s="177"/>
+      <c r="Q8" s="157"/>
+      <c r="R8" s="187"/>
+      <c r="S8" s="185"/>
+      <c r="T8" s="187"/>
+      <c r="U8" s="187"/>
+      <c r="V8" s="187"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="40"/>
@@ -48428,16 +48428,12 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="R7:R8"/>
     <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="S4:S5"/>
     <mergeCell ref="B6:C6"/>
@@ -48454,12 +48450,16 @@
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <dataValidations count="26">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Besvaras bara med Ja eller Nej" promptTitle="Kvalifikation" prompt="Läs instruktion för kvalifikation. Välj om deltagare erhållit någon formell kvalifikation." sqref="S10 S40 S70 S100 S130 S160 S190 S220 S250 S381 S411 S441 S471 S501 S531 S561 S590 S636 S665 S292 S322 S352 S713 S743 S773 S803 S833 S863 S892 S938 S967">
@@ -48557,8 +48557,8 @@
   </sheetPr>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:E2"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A16" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48574,29 +48574,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="188" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
-      <c r="D1" s="197"/>
-      <c r="E1" s="197"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
     </row>
     <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="197"/>
-      <c r="B2" s="197"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
+      <c r="A2" s="188"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="198" t="s">
+      <c r="A3" s="189" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="198"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="198"/>
+      <c r="B3" s="189"/>
+      <c r="C3" s="189"/>
+      <c r="D3" s="189"/>
+      <c r="E3" s="189"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="107"/>
@@ -48675,12 +48675,12 @@
       <c r="E11" s="116"/>
     </row>
     <row r="12" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="199" t="s">
+      <c r="A12" s="190" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="200"/>
-      <c r="C12" s="200"/>
-      <c r="D12" s="201"/>
+      <c r="B12" s="191"/>
+      <c r="C12" s="191"/>
+      <c r="D12" s="192"/>
       <c r="E12" s="109"/>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -48690,22 +48690,22 @@
       <c r="B13" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="202" t="s">
+      <c r="C13" s="193" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="203"/>
+      <c r="D13" s="194"/>
       <c r="E13" s="109"/>
     </row>
     <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="204" t="s">
+      <c r="A14" s="195" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="205"/>
-      <c r="C14" s="206">
+      <c r="B14" s="196"/>
+      <c r="C14" s="197">
         <f>Deltagarförteckning!H1010</f>
         <v>0</v>
       </c>
-      <c r="D14" s="207"/>
+      <c r="D14" s="198"/>
       <c r="E14" s="109"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -48723,10 +48723,10 @@
       <c r="E16" s="109"/>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="190" t="s">
+      <c r="A17" s="199" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="190"/>
+      <c r="B17" s="199"/>
       <c r="C17" s="121">
         <f>COUNTIF(Deltagarförteckning!M9:M1009,"&gt;0")</f>
         <v>0</v>
@@ -48735,10 +48735,10 @@
       <c r="E17" s="109"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="190" t="s">
+      <c r="A18" s="199" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="190"/>
+      <c r="B18" s="199"/>
       <c r="C18" s="121">
         <f>Deltagarförteckning!J1010</f>
         <v>0</v>
@@ -48747,10 +48747,10 @@
       <c r="E18" s="109"/>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="195" t="s">
+      <c r="A19" s="200" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="195"/>
+      <c r="B19" s="200"/>
       <c r="C19" s="121">
         <f>SUM(Deltagarförteckning!H1010)</f>
         <v>0</v>
@@ -48759,17 +48759,17 @@
       <c r="E19" s="109"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="196"/>
-      <c r="B20" s="196"/>
-      <c r="C20" s="196"/>
-      <c r="D20" s="196"/>
+      <c r="A20" s="201"/>
+      <c r="B20" s="201"/>
+      <c r="C20" s="201"/>
+      <c r="D20" s="201"/>
       <c r="E20" s="109"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="195" t="s">
+      <c r="A21" s="200" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="195"/>
+      <c r="B21" s="200"/>
       <c r="C21" s="122" t="str">
         <f>IFERROR(C19/C17,"")</f>
         <v/>
@@ -48778,10 +48778,10 @@
       <c r="E21" s="109"/>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="195" t="s">
+      <c r="A22" s="200" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="195"/>
+      <c r="B22" s="200"/>
       <c r="C22" s="122" t="str">
         <f>IFERROR(C19/C18,"")</f>
         <v/>
@@ -48790,10 +48790,10 @@
       <c r="E22" s="109"/>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="190" t="s">
+      <c r="A23" s="199" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="190"/>
+      <c r="B23" s="199"/>
       <c r="C23" s="123">
         <f>COUNTIF(Deltagarförteckning!E9:E1009,"=K")</f>
         <v>0</v>
@@ -48802,10 +48802,10 @@
       <c r="E23" s="109"/>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="190" t="s">
+      <c r="A24" s="199" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="190"/>
+      <c r="B24" s="199"/>
       <c r="C24" s="123">
         <f>COUNTIF(Deltagarförteckning!E9:E1009,"=M")</f>
         <v>0</v>
@@ -48823,10 +48823,10 @@
       <c r="E25" s="109"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="190" t="s">
+      <c r="A26" s="199" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="190"/>
+      <c r="B26" s="199"/>
       <c r="C26" s="123" t="str">
         <f ca="1">IF(Data!J1=0,"",Data!J1)</f>
         <v/>
@@ -48835,10 +48835,10 @@
       <c r="E26" s="109"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="190" t="s">
+      <c r="A27" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="190"/>
+      <c r="B27" s="199"/>
       <c r="C27" s="123" t="str">
         <f>IF(Data!J2=0,"",Data!J2)</f>
         <v/>
@@ -48847,10 +48847,10 @@
       <c r="E27" s="109"/>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="190" t="s">
+      <c r="A28" s="199" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="190"/>
+      <c r="B28" s="199"/>
       <c r="C28" s="123" t="str">
         <f>IF(Data!J3=0,"",Data!J3)</f>
         <v/>
@@ -48859,10 +48859,10 @@
       <c r="E28" s="109"/>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="190" t="s">
+      <c r="A29" s="199" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="190"/>
+      <c r="B29" s="199"/>
       <c r="C29" s="123" t="str">
         <f>IF(Data!J4=0,"",Data!J4)</f>
         <v/>
@@ -48871,10 +48871,10 @@
       <c r="E29" s="109"/>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="190" t="s">
+      <c r="A30" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="190"/>
+      <c r="B30" s="199"/>
       <c r="C30" s="123" t="str">
         <f>IF(Data!J5=0,"",Data!J5)</f>
         <v/>
@@ -48883,10 +48883,10 @@
       <c r="E30" s="109"/>
     </row>
     <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="190" t="s">
+      <c r="A31" s="199" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="190"/>
+      <c r="B31" s="199"/>
       <c r="C31" s="123" t="str">
         <f>IF(Data!J6=0,"",Data!J6)</f>
         <v/>
@@ -48895,10 +48895,10 @@
       <c r="E31" s="109"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="190" t="s">
+      <c r="A32" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="190"/>
+      <c r="B32" s="199"/>
       <c r="C32" s="123" t="str">
         <f>IF(Data!J7=0,"",Data!J7)</f>
         <v/>
@@ -48908,7 +48908,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="127" t="str">
-        <f ca="1">IF(Data!J10=0,"","Typ av organisation saknas på en eller flera aktörer se flik Register_deltag_organisationer")</f>
+        <f ca="1">IF(Data!J10&lt;1,"","Typ av organisation saknas på en eller flera aktörer se flik Register_deltag_organisationer")</f>
         <v/>
       </c>
       <c r="B33" s="128"/>
@@ -48917,12 +48917,12 @@
       <c r="E33" s="109"/>
     </row>
     <row r="34" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="191" t="s">
+      <c r="A34" s="204" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="191"/>
-      <c r="C34" s="191"/>
-      <c r="D34" s="191"/>
+      <c r="B34" s="204"/>
+      <c r="C34" s="204"/>
+      <c r="D34" s="204"/>
       <c r="E34" s="131"/>
       <c r="F34" s="132"/>
       <c r="G34" s="132"/>
@@ -48946,28 +48946,28 @@
         <v>87</v>
       </c>
       <c r="B37" s="109"/>
-      <c r="C37" s="192" t="s">
+      <c r="C37" s="205" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="192"/>
+      <c r="D37" s="205"/>
       <c r="E37" s="109"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="193" t="s">
+      <c r="A38" s="206" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="193"/>
-      <c r="C38" s="194" t="s">
+      <c r="B38" s="206"/>
+      <c r="C38" s="207" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="194"/>
+      <c r="D38" s="207"/>
       <c r="E38" s="109"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="188" t="s">
+      <c r="A39" s="202" t="s">
         <v>91</v>
       </c>
-      <c r="B39" s="188"/>
+      <c r="B39" s="202"/>
       <c r="C39" s="109"/>
       <c r="D39" s="109"/>
       <c r="E39" s="109"/>
@@ -48987,27 +48987,27 @@
       <c r="E41" s="109"/>
     </row>
     <row r="42" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="189" t="s">
+      <c r="A42" s="203" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="189"/>
-      <c r="C42" s="189"/>
-      <c r="D42" s="189"/>
+      <c r="B42" s="203"/>
+      <c r="C42" s="203"/>
+      <c r="D42" s="203"/>
       <c r="E42" s="136"/>
       <c r="F42" s="137"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="189"/>
-      <c r="B43" s="189"/>
-      <c r="C43" s="189"/>
-      <c r="D43" s="189"/>
+      <c r="A43" s="203"/>
+      <c r="B43" s="203"/>
+      <c r="C43" s="203"/>
+      <c r="D43" s="203"/>
       <c r="E43" s="109"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="189"/>
-      <c r="B44" s="189"/>
-      <c r="C44" s="189"/>
-      <c r="D44" s="189"/>
+      <c r="A44" s="203"/>
+      <c r="B44" s="203"/>
+      <c r="C44" s="203"/>
+      <c r="D44" s="203"/>
       <c r="E44" s="109"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -49062,12 +49062,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A42:D44"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
@@ -49080,17 +49083,14 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A42:D44"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Projektrelaterad tid" error="- Bara projektrelaterade timmar registreras i blanketten. _x000a__x000a_Klicka på avbryt eller försök igen för att gå tillbaka och ändra._x000a_" sqref="C17 C33"/>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0" top="1.3779527559055118" bottom="0.19685039370078741" header="0.59055118110236227" footer="0.31496062992125984"/>
@@ -49104,7 +49104,7 @@
   <legacyDrawingHF r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
             <xm:f>Data!#REF!</xm:f>

</xml_diff>